<commit_message>
make datasource extends sqlite
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -579,7 +579,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-01</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -618,7 +618,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-01</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -657,7 +657,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>2023-11-01</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -696,7 +696,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -774,7 +774,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -813,7 +813,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -852,7 +852,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-03</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -891,7 +891,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-03</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -930,7 +930,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-04</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-05</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>2023-11-09</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>2023-11-09</t>
         </is>
       </c>
       <c r="D23" t="n">

</xml_diff>

<commit_message>
move main.py to root
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -618,7 +618,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -657,7 +657,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>2023-11-03</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -696,7 +696,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-04</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-04</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -774,7 +774,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-04</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -813,7 +813,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-05</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -852,7 +852,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -891,7 +891,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -930,7 +930,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-11-04</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -969,7 +969,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-09</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="D23" t="n">

</xml_diff>